<commit_message>
Update CSEN603 - RequirementsTemplateM1.xlsx
Added Team Info
</commit_message>
<xml_diff>
--- a/CSEN603 - RequirementsTemplateM1.xlsx
+++ b/CSEN603 - RequirementsTemplateM1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahmoud\Documents\GitHub\dora-the-explorer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\dora-the-explorer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA97124-32A0-429A-BD44-5E907DA3F62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C9AF92-F5D9-4EA2-9CBF-084F786645DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Info" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Team Name</t>
   </si>
@@ -95,12 +95,69 @@
   <si>
     <t>Students</t>
   </si>
+  <si>
+    <t>Mohamed Gamal</t>
+  </si>
+  <si>
+    <t>55-12064</t>
+  </si>
+  <si>
+    <t>mohamed.gamal@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>Youssef Sherif Sabry Fawzy</t>
+  </si>
+  <si>
+    <t>55-6528</t>
+  </si>
+  <si>
+    <t>youssef.fawzy@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>Mahmoud Hegazy</t>
+  </si>
+  <si>
+    <t>55-13845</t>
+  </si>
+  <si>
+    <t>mahmod.hegazy@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>John Elkess Antonious</t>
+  </si>
+  <si>
+    <t>55-4548</t>
+  </si>
+  <si>
+    <t>john.edward@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>T-26</t>
+  </si>
+  <si>
+    <t>T-10</t>
+  </si>
+  <si>
+    <t>T-18</t>
+  </si>
+  <si>
+    <t>Hazem Essam Brekaa</t>
+  </si>
+  <si>
+    <t>55-15850</t>
+  </si>
+  <si>
+    <t>hazem.brekaa@student.guc.edu.eg</t>
+  </si>
+  <si>
+    <t>T-11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -190,6 +247,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -235,10 +299,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -293,8 +358,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,8 +580,8 @@
   </sheetPr>
   <dimension ref="A1:D998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -572,34 +639,74 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -1599,8 +1706,11 @@
     <mergeCell ref="A2:D4"/>
     <mergeCell ref="A5:D5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{FB6B7E0C-502F-4915-9BE5-6F0C84B87A95}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1611,8 +1721,8 @@
   </sheetPr>
   <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2877,7 +2987,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>